<commit_message>
output for manually coding crimes
</commit_message>
<xml_diff>
--- a/01-preprocess/judicial/codebook_judiciales.xlsx
+++ b/01-preprocess/judicial/codebook_judiciales.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\Prisions\code\01-preprocess\judicial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC483BBA-B867-4D3B-8BE2-8B02885CA1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C448608B-C9A7-4E74-A64A-FD0721CFCBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{98A18676-1530-40A9-A98D-A7BE4F6AEA8C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{98A18676-1530-40A9-A98D-A7BE4F6AEA8C}"/>
   </bookViews>
   <sheets>
     <sheet name="2000-2008" sheetId="1" r:id="rId1"/>
-    <sheet name="2008-2012" sheetId="2" r:id="rId2"/>
+    <sheet name="2009-2012" sheetId="2" r:id="rId2"/>
     <sheet name="2014-2020" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Bases</t>
   </si>
@@ -45,14 +45,193 @@
   </si>
   <si>
     <t>SREGyear.DBF</t>
+  </si>
+  <si>
+    <t>Datos sobre sentencias, etc</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>var_name</t>
+  </si>
+  <si>
+    <t>Id_ps</t>
+  </si>
+  <si>
+    <t>ID processed</t>
+  </si>
+  <si>
+    <t>B_cvestad</t>
+  </si>
+  <si>
+    <t>var_analysis</t>
+  </si>
+  <si>
+    <t>fuero (federal 42, comun 41)</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>merges</t>
+  </si>
+  <si>
+    <t>B_mesreg</t>
+  </si>
+  <si>
+    <t>month of register</t>
+  </si>
+  <si>
+    <t>B_anoreg</t>
+  </si>
+  <si>
+    <t>year of register</t>
+  </si>
+  <si>
+    <t>outcome: date of sentence - date of register: total days the case was revised</t>
+  </si>
+  <si>
+    <t>B_entreg</t>
+  </si>
+  <si>
+    <t>B_munreg</t>
+  </si>
+  <si>
+    <t>State register</t>
+  </si>
+  <si>
+    <t>Mun register</t>
+  </si>
+  <si>
+    <t>check for differences in register and municipality and crime done</t>
+  </si>
+  <si>
+    <t>B_entnac</t>
+  </si>
+  <si>
+    <t>B_munnac</t>
+  </si>
+  <si>
+    <t>B_entrh</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>check for Nas</t>
+  </si>
+  <si>
+    <t>B_munrh</t>
+  </si>
+  <si>
+    <t>treatment (distance to closest center)</t>
+  </si>
+  <si>
+    <t>State birth</t>
+  </si>
+  <si>
+    <t>Mun birth</t>
+  </si>
+  <si>
+    <t>State residence</t>
+  </si>
+  <si>
+    <t>Mun residence</t>
+  </si>
+  <si>
+    <t>B_totdel</t>
+  </si>
+  <si>
+    <t>Total crimes</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>B_fauto</t>
+  </si>
+  <si>
+    <t>date of sentence</t>
+  </si>
+  <si>
+    <t>B_numdel</t>
+  </si>
+  <si>
+    <t>Number of crime</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>B_fuero</t>
+  </si>
+  <si>
+    <t>Fuero crime (1 común, 2 federal)</t>
+  </si>
+  <si>
+    <t>B_grave</t>
+  </si>
+  <si>
+    <t>maybe to distinguish petty crimes from harsh ones?</t>
+  </si>
+  <si>
+    <t>B_entoc</t>
+  </si>
+  <si>
+    <t>B_munoc</t>
+  </si>
+  <si>
+    <t>State crime commited</t>
+  </si>
+  <si>
+    <t>Municipality crime commited</t>
+  </si>
+  <si>
+    <t>B_auto</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Important crime (stay with True)</t>
+  </si>
+  <si>
+    <t>Judicial resolution (72 hours after process) (1: irregular process, 2: prison, 3: sujeción a proceso, 4: no sujecion a proceso, 5: provisional reclusión, 6: absolute liberty)</t>
+  </si>
+  <si>
+    <t>two variables: sentenced on the spot (72 hours) or sent to preventive prison</t>
+  </si>
+  <si>
+    <t>Seriousness (grave 1, no grave 2, no especificada 9)</t>
+  </si>
+  <si>
+    <t>could be repeated if crimes &gt; 1, so first pivot wider</t>
+  </si>
+  <si>
+    <t>Datos generales y demograficos de los procesados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos generales y demograficos de los sentenciados. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,7 +247,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -76,12 +255,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0192BBF5-57F9-4F05-AFBE-DFA9207890B6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,6 +622,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -440,17 +633,316 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40746ADF-322E-4B37-933A-99567471DA4E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>